<commit_message>
adding 4 more resultt and new charts
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Parsa\Desktop\Study materials\3D Computer vision\Point Registration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A276EFAD-22EC-4CFA-9823-0BE45DC57C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7769BED0-F6E7-465B-8020-EC40B6D194E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>ICP Error</t>
   </si>
@@ -122,6 +122,18 @@
   <si>
     <t>Error</t>
   </si>
+  <si>
+    <t>Aloe Guassian noise 0.2 std</t>
+  </si>
+  <si>
+    <t>Aloe Guassian noise 0.05 std</t>
+  </si>
+  <si>
+    <t>Aloe Guassian noise and rotate 5</t>
+  </si>
+  <si>
+    <t>Aloe Guassian noise and rotate 10</t>
+  </si>
 </sst>
 </file>
 
@@ -144,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,12 +164,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1696,102 +1724,162 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$6</c:f>
+              <c:f>Sheet1!$D$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Tr-ICP MSE Error</c:v>
+                  <c:v>ICP Runtime</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:yVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$7:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>fountain_a</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gaussian noise fountain_a mean=0 std=0.1 </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fountain_a.xyz_Rotated 5 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>fountain_a.xyz_Rotated 10 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>p1_Aloe</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>p1_Aloe_Rotated 5 Over x axis </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>p1_Aloe_Rotated 10 Over x axis </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>p1_Aloe_Rotated 15 Over x axis </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Gaussian noise p1_Aloe mean=0 std=0.1 </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>p1_Baby</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>p1_Baby_Rotated 5 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>p1_Baby_Rotated 10 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>p1_Baby_Rotated 15 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Gaussian noise p1_Baby mean=0 std=0.1 </c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Aloe Guassian noise 0.2 std</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Aloe Guassian noise 0.05 std</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Aloe Guassian noise and rotate 5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Aloe Guassian noise and rotate 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$7:$G$20</c:f>
+              <c:f>Sheet1!$D$7:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>9.9050100000000006E-3</c:v>
+                  <c:v>19.346900000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6034099999999999E-2</c:v>
+                  <c:v>58.2669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0069699999999999E-2</c:v>
+                  <c:v>47.953800000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.13624E-2</c:v>
+                  <c:v>24.096399999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74.562700000000007</c:v>
+                  <c:v>53.997900000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74.571899999999999</c:v>
+                  <c:v>70.448899999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>74.571899999999999</c:v>
+                  <c:v>37.249000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>74.571899999999999</c:v>
+                  <c:v>73.946299999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>74.572299999999998</c:v>
+                  <c:v>83.446799999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42.318300000000001</c:v>
+                  <c:v>35.651200000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42.318600000000004</c:v>
+                  <c:v>54.128300000000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42.316699999999997</c:v>
+                  <c:v>69.234499999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46.615200000000002</c:v>
+                  <c:v>63.558500000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42.316899999999997</c:v>
+                  <c:v>79.859300000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>89.846100000000007</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>66.561000000000007</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>104.10899999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128.678</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B4DF-45E3-B9FC-7399D7C7C7D6}"/>
+              <c16:uniqueId val="{00000000-7C06-47DC-8D37-9BA473562709}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1803,30 +1891,19 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="594076991"/>
-        <c:axId val="594076575"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="594076991"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1977671872"/>
+        <c:axId val="1977670624"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1977671872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1835,8 +1912,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1863,12 +1940,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="594076575"/>
+        <c:crossAx val="1977670624"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="594076575"/>
+        <c:axId val="1977670624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1894,14 +1974,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1925,9 +1999,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="594076991"/>
+        <c:crossAx val="1977671872"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2021,8 +2095,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2039,23 +2114,83 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$7:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>fountain_a</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gaussian noise fountain_a mean=0 std=0.1 </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fountain_a.xyz_Rotated 5 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>fountain_a.xyz_Rotated 10 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>p1_Aloe</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>p1_Aloe_Rotated 5 Over x axis </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>p1_Aloe_Rotated 10 Over x axis </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>p1_Aloe_Rotated 15 Over x axis </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Gaussian noise p1_Aloe mean=0 std=0.1 </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>p1_Baby</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>p1_Baby_Rotated 5 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>p1_Baby_Rotated 10 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>p1_Baby_Rotated 15 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Gaussian noise p1_Baby mean=0 std=0.1 </c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Aloe Guassian noise 0.2 std</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Aloe Guassian noise 0.05 std</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Aloe Guassian noise and rotate 5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Aloe Guassian noise and rotate 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$7:$F$20</c:f>
+              <c:f>Sheet1!$F$7:$F$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>3.5268299999999999</c:v>
                 </c:pt>
@@ -2097,14 +2232,25 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>135.738</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>148.07499999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>156.364</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>156.33000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>128.96299999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FD48-4048-8980-0BC9FCC25BBB}"/>
+              <c16:uniqueId val="{00000000-9712-4A5B-8F7D-65E58848F2AB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2116,12 +2262,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="427770639"/>
-        <c:axId val="427771055"/>
-      </c:lineChart>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1977658144"/>
+        <c:axId val="1977651488"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="427770639"/>
+        <c:axId val="1977658144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2164,7 +2311,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427771055"/>
+        <c:crossAx val="1977651488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2172,7 +2319,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="427771055"/>
+        <c:axId val="1977651488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2223,7 +2370,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="427770639"/>
+        <c:crossAx val="1977658144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2319,90 +2466,162 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$6</c:f>
+              <c:f>Sheet1!$E$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Tr-ICP MSE Error</c:v>
+                  <c:v>ICP Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$7:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>fountain_a</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gaussian noise fountain_a mean=0 std=0.1 </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fountain_a.xyz_Rotated 5 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>fountain_a.xyz_Rotated 10 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>p1_Aloe</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>p1_Aloe_Rotated 5 Over x axis </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>p1_Aloe_Rotated 10 Over x axis </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>p1_Aloe_Rotated 15 Over x axis </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Gaussian noise p1_Aloe mean=0 std=0.1 </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>p1_Baby</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>p1_Baby_Rotated 5 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>p1_Baby_Rotated 10 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>p1_Baby_Rotated 15 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Gaussian noise p1_Baby mean=0 std=0.1 </c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Aloe Guassian noise 0.2 std</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Aloe Guassian noise 0.05 std</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Aloe Guassian noise and rotate 5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Aloe Guassian noise and rotate 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$7:$G$20</c:f>
+              <c:f>Sheet1!$E$7:$E$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>9.9050100000000006E-3</c:v>
+                  <c:v>0.270897</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6034099999999999E-2</c:v>
+                  <c:v>0.26137700000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0069699999999999E-2</c:v>
+                  <c:v>0.25117200000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.13624E-2</c:v>
+                  <c:v>0.270625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>74.562700000000007</c:v>
+                  <c:v>15.7857</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74.571899999999999</c:v>
+                  <c:v>15.786</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>74.571899999999999</c:v>
+                  <c:v>15.793699999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>74.571899999999999</c:v>
+                  <c:v>15.785600000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>74.572299999999998</c:v>
+                  <c:v>15.786799999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42.318300000000001</c:v>
+                  <c:v>12.501899999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42.318600000000004</c:v>
+                  <c:v>12.513400000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42.316699999999997</c:v>
+                  <c:v>12.5152</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46.615200000000002</c:v>
+                  <c:v>12.5146</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42.316899999999997</c:v>
+                  <c:v>12.513400000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27.070499999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27.066099999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27.0761</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27.079699999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FFB1-4855-9F25-56E6770E6461}"/>
+              <c16:uniqueId val="{00000000-9A64-41DE-8321-31A1D53583E4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2414,17 +2633,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="602557727"/>
-        <c:axId val="602548575"/>
-      </c:lineChart>
+        <c:gapWidth val="182"/>
+        <c:axId val="1993084672"/>
+        <c:axId val="1993075104"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="602557727"/>
+        <c:axId val="1993084672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2462,7 +2681,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="602548575"/>
+        <c:crossAx val="1993075104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2470,12 +2689,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="602548575"/>
+        <c:axId val="1993075104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2521,7 +2740,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="602557727"/>
+        <c:crossAx val="1993084672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2617,90 +2836,162 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$6</c:f>
+              <c:f>Sheet1!$G$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ICP Runtime</c:v>
+                  <c:v>Tr-ICP MSE Error</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$7:$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>fountain_a</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Gaussian noise fountain_a mean=0 std=0.1 </c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fountain_a.xyz_Rotated 5 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>fountain_a.xyz_Rotated 10 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>p1_Aloe</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>p1_Aloe_Rotated 5 Over x axis </c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>p1_Aloe_Rotated 10 Over x axis </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>p1_Aloe_Rotated 15 Over x axis </c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Gaussian noise p1_Aloe mean=0 std=0.1 </c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>p1_Baby</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>p1_Baby_Rotated 5 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>p1_Baby_Rotated 10 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>p1_Baby_Rotated 15 Over Z axis</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Gaussian noise p1_Baby mean=0 std=0.1 </c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Aloe Guassian noise 0.2 std</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Aloe Guassian noise 0.05 std</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Aloe Guassian noise and rotate 5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Aloe Guassian noise and rotate 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$7:$D$20</c:f>
+              <c:f>Sheet1!$G$7:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>19.346900000000002</c:v>
+                  <c:v>9.9050100000000006E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58.2669</c:v>
+                  <c:v>1.6034099999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47.953800000000001</c:v>
+                  <c:v>1.0069699999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.096399999999999</c:v>
+                  <c:v>1.13624E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53.997900000000001</c:v>
+                  <c:v>74.562700000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70.448899999999995</c:v>
+                  <c:v>74.571899999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>37.249000000000002</c:v>
+                  <c:v>74.571899999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>73.946299999999994</c:v>
+                  <c:v>74.571899999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>83.446799999999996</c:v>
+                  <c:v>74.572299999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>35.651200000000003</c:v>
+                  <c:v>42.318300000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>54.128300000000003</c:v>
+                  <c:v>42.318600000000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>69.234499999999997</c:v>
+                  <c:v>42.316699999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>63.558500000000002</c:v>
+                  <c:v>46.615200000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>49.859299999999998</c:v>
+                  <c:v>42.316899999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>276.90199999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>276.86900000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>276.87700000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>325.86200000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-95F9-48A3-A118-9AD89C09E91B}"/>
+              <c16:uniqueId val="{00000000-A4E2-4818-8617-7CF844E2EEB0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2712,17 +3003,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="598397071"/>
-        <c:axId val="598397903"/>
-      </c:lineChart>
+        <c:gapWidth val="182"/>
+        <c:axId val="1993067200"/>
+        <c:axId val="1993069696"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="598397071"/>
+        <c:axId val="1993067200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2760,7 +3051,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="598397903"/>
+        <c:crossAx val="1993069696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2768,12 +3059,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="598397903"/>
+        <c:axId val="1993069696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2819,7 +3110,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="598397071"/>
+        <c:crossAx val="1993067200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2986,6 +3277,43 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3025,48 +3353,11 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
-  <a:schemeClr val="accent2"/>
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -4132,7 +4423,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4159,8 +4450,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4261,7 +4552,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4293,10 +4584,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4336,23 +4627,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -4457,8 +4747,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4590,20 +4880,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4617,17 +4906,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4648,7 +4926,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4756,11 +5034,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -4771,11 +5044,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -4807,9 +5075,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5164,7 +5429,7 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5272,11 +5537,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -5287,11 +5547,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -5323,9 +5578,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5381,22 +5633,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5501,8 +5754,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5634,19 +5887,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5680,7 +5934,7 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5788,11 +6042,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -5803,11 +6052,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -5839,9 +6083,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5897,22 +6138,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -6017,8 +6259,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6150,19 +6392,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -6207,7 +6450,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6237,13 +6480,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>420221</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>146796</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>151280</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>32496</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6271,23 +6514,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>329045</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>146796</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>521073</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>32496</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0339670E-A972-4DA7-9D79-F1F97D5EEB6C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{193F6A82-4EEF-4A31-901E-B8AE0C41931B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6307,23 +6550,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>346363</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>124385</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>487455</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>10085</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E42A910-EB30-4BF8-A842-850D91C36312}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E706B7E4-B761-49E1-9BD6-907AFAE5521A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6343,23 +6586,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>156881</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142009</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>27274</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>259772</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>166966</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>346363</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>173181</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AE6185C-32F6-4E49-8FB3-1C6FCA0E97B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE92155F-4425-4DAA-B18E-1E0A1FCA421D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6379,23 +6622,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>16809</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>113178</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>121227</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>83127</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>229721</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>189378</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>346362</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>69273</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9">
+        <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2279DA64-4F9E-4515-BE4E-952B3B8F9753}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74170743-8DC5-4DC9-A2B8-AF7C82A87CBF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6681,8 +6924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A6:L200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J126" sqref="J126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7112,7 +7355,7 @@
         <v>23</v>
       </c>
       <c r="D20">
-        <v>49.859299999999998</v>
+        <v>79.859300000000005</v>
       </c>
       <c r="E20">
         <v>12.513400000000001</v>
@@ -7131,6 +7374,27 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21">
+        <v>89.846100000000007</v>
+      </c>
+      <c r="E21">
+        <v>27.070499999999999</v>
+      </c>
+      <c r="F21">
+        <v>148.07499999999999</v>
+      </c>
+      <c r="G21">
+        <v>276.90199999999999</v>
+      </c>
       <c r="K21">
         <v>17.5822</v>
       </c>
@@ -7139,6 +7403,27 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <v>66.561000000000007</v>
+      </c>
+      <c r="E22">
+        <v>27.066099999999999</v>
+      </c>
+      <c r="F22">
+        <v>156.364</v>
+      </c>
+      <c r="G22">
+        <v>276.86900000000003</v>
+      </c>
       <c r="K22">
         <v>17.294499999999999</v>
       </c>
@@ -7147,11 +7432,26 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
       <c r="C23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" t="s">
-        <v>28</v>
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>104.10899999999999</v>
+      </c>
+      <c r="E23">
+        <v>27.0761</v>
+      </c>
+      <c r="F23">
+        <v>156.33000000000001</v>
+      </c>
+      <c r="G23">
+        <v>276.87700000000001</v>
       </c>
       <c r="K23">
         <v>17.029900000000001</v>
@@ -7161,16 +7461,26 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>18</v>
+      </c>
       <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24">
-        <f>AVERAGE(D7:D20)</f>
-        <v>52.941764285714285</v>
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
       </c>
       <c r="D24">
-        <f>AVERAGE(E7:E20)</f>
-        <v>10.182169357142858</v>
+        <v>128.678</v>
+      </c>
+      <c r="E24">
+        <v>27.079699999999999</v>
+      </c>
+      <c r="F24">
+        <v>128.96299999999999</v>
+      </c>
+      <c r="G24">
+        <v>325.86200000000002</v>
       </c>
       <c r="K24">
         <v>16.719200000000001</v>
@@ -7180,17 +7490,6 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25">
-        <f>AVERAGE(F7:F20)</f>
-        <v>41.559115714285717</v>
-      </c>
-      <c r="D25">
-        <f>AVERAGE(G7:G20)</f>
-        <v>42.055983657857141</v>
-      </c>
       <c r="K25">
         <v>16.310099999999998</v>
       </c>
@@ -7231,6 +7530,13 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="K30">
         <v>14.2463</v>
       </c>
@@ -7239,6 +7545,17 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="1">
+        <f>AVERAGE(D7:D24)</f>
+        <v>64.465488888888885</v>
+      </c>
+      <c r="D31" s="1">
+        <f>AVERAGE(E7:E24)</f>
+        <v>13.935709500000002</v>
+      </c>
       <c r="K31">
         <v>14.037800000000001</v>
       </c>
@@ -7247,6 +7564,17 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="1">
+        <f>AVERAGE(F7:F24)</f>
+        <v>65.086645555555549</v>
+      </c>
+      <c r="D32" s="1">
+        <f>AVERAGE(G7:G24)</f>
+        <v>96.960765067222226</v>
+      </c>
       <c r="K32">
         <v>13.866</v>
       </c>

</xml_diff>